<commit_message>
GDE-8218 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE8C681-34D3-47A9-B7DC-EBAB1FE1BA08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEFD243-788A-46FC-8344-AD944FEBA162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="7830" tabRatio="923" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="7830" tabRatio="923" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="865">
   <si>
     <t>rowid</t>
   </si>
@@ -2641,6 +2641,9 @@
   </si>
   <si>
     <t>John Bloggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -4279,9 +4282,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AP14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4579,6 +4584,11 @@
       </c>
       <c r="AP2" s="86" t="s">
         <v>769</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="I14" s="86" t="s">
+        <v>864</v>
       </c>
     </row>
   </sheetData>
@@ -8662,7 +8672,7 @@
   </sheetPr>
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D6" sqref="D6"/>
     </sheetView>

</xml_diff>

<commit_message>
GDE-8220 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="885" windowWidth="28800" windowHeight="7830" tabRatio="923" firstSheet="2" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1423,8 +1423,8 @@
     <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="7" max="7"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="88" min="8" max="8"/>
     <col width="20.5703125" customWidth="1" style="88" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="88" min="10" max="26"/>
-    <col width="8.7109375" customWidth="1" style="88" min="27" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="10" max="28"/>
+    <col width="8.7109375" customWidth="1" style="88" min="29" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -1480,19 +1480,19 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EVG_S4_EU_NonRPA_Branch</t>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
         </is>
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>S4_NONRPA_29102020131303KCE</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>S4_NONRPA_29102020131303KCE</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="H2" s="88" t="inlineStr">
@@ -1546,8 +1546,8 @@
   </sheetPr>
   <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1820,15 +1820,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EVG_S4_EU_NonRPA_Branch</t>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
         </is>
       </c>
       <c r="C2" s="31" t="n"/>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="E2" s="15" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>S4_NONRPA_29102020131303KCE</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="G2" s="103" t="inlineStr">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>S4_NONRPA_29102020131303KCE</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="M2" s="86" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="S2" s="86" t="inlineStr">
         <is>
-          <t>07-Aug-2025</t>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="T2" s="15" t="inlineStr">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="I2" s="86" t="inlineStr">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="S2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="T2" s="86" t="inlineStr">
@@ -4181,8 +4181,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="80"/>
-    <col width="9.140625" customWidth="1" style="68" min="81" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="82"/>
+    <col width="9.140625" customWidth="1" style="68" min="83" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -6874,8 +6874,8 @@
   <dimension ref="A1:CY2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP19" sqref="AP19"/>
+      <pane xSplit="2" topLeftCell="BB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BI7" sqref="BI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7518,17 +7518,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_05112020175500TLP</t>
+          <t>R5_06112020154352RZL</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_05112020181207ELY</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -7737,7 +7737,7 @@
       </c>
       <c r="BD2" s="5" t="inlineStr">
         <is>
-          <t>Commitment Fee</t>
+          <t>Usage Fee</t>
         </is>
       </c>
       <c r="BE2" s="5" t="inlineStr">
@@ -7954,7 +7954,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8004,7 +8004,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -8014,7 +8014,7 @@
     <col width="21.7109375" customWidth="1" style="86" min="3" max="3"/>
     <col width="19.5703125" customWidth="1" style="86" min="4" max="4"/>
     <col width="43.85546875" bestFit="1" customWidth="1" style="86" min="5" max="5"/>
-    <col width="29" bestFit="1" customWidth="1" style="86" min="6" max="6"/>
+    <col width="34.140625" bestFit="1" customWidth="1" style="86" min="6" max="6"/>
     <col width="22.85546875" customWidth="1" style="86" min="7" max="7"/>
     <col width="14.42578125" customWidth="1" style="86" min="8" max="8"/>
     <col width="14.5703125" customWidth="1" style="86" min="9" max="9"/>
@@ -8226,12 +8226,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_05112020181207ELY</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -8254,9 +8254,24 @@
           <t>EUR</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>03-Nov-2020</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>03-Nov-2020</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>03-Nov-2025</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="R2" s="86" t="inlineStr">
@@ -8341,11 +8356,11 @@
   </sheetPr>
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="V22" sqref="V22"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -8497,7 +8512,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_05112020181207ELY</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8507,7 +8522,7 @@
       </c>
       <c r="E2" s="22" t="inlineStr">
         <is>
-          <t>Commitment Fee</t>
+          <t>Usage Fee</t>
         </is>
       </c>
       <c r="F2" s="5" t="inlineStr">
@@ -8646,7 +8661,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8919,19 +8934,19 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EVG_S4_EU_NonRPA_Branch</t>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_05112020181207ELY</t>
+          <t>R5_BYBK_100M_06112020160123XRR</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -9003,6 +9018,11 @@
       <c r="S2" s="5" t="inlineStr">
         <is>
           <t>100</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>03-Nov-2025</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -9056,7 +9076,7 @@
       <c r="A3" s="46" t="n"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="L3" s="46" t="n"/>
@@ -9071,7 +9091,7 @@
       <c r="A4" s="46" t="n"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="L4" s="46" t="n"/>
@@ -9098,8 +9118,8 @@
   </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9216,14 +9236,14 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EVG_S4_EU_NonRPA_Branch</t>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_05112020175457UDX</t>
+          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
         </is>
       </c>
       <c r="D2" s="84" t="inlineStr">

</xml_diff>

<commit_message>
GDE-8221 - Initial Commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="885" windowWidth="28800" windowHeight="7830" tabRatio="923" firstSheet="2" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,15 +17,16 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED07_UpfrontFee_Payment" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_ExternalParticipation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -298,7 +299,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -452,6 +453,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,14 +1419,14 @@
     <col width="5.85546875" bestFit="1" customWidth="1" style="88" min="1" max="1"/>
     <col width="28" bestFit="1" customWidth="1" style="88" min="2" max="2"/>
     <col width="44" bestFit="1" customWidth="1" style="88" min="3" max="3"/>
-    <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="4" max="4"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="88" min="4" max="4"/>
     <col width="21.7109375" customWidth="1" style="88" min="5" max="5"/>
     <col width="26.28515625" bestFit="1" customWidth="1" style="88" min="6" max="6"/>
     <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="7" max="7"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="88" min="8" max="8"/>
     <col width="20.5703125" customWidth="1" style="88" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="88" min="10" max="28"/>
-    <col width="8.7109375" customWidth="1" style="88" min="29" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="10" max="33"/>
+    <col width="8.7109375" customWidth="1" style="88" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -1487,12 +1489,12 @@
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -1507,7 +1509,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="88" t="inlineStr">
@@ -1521,7 +1523,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="46" t="n"/>
       <c r="B4" s="86" t="n"/>
@@ -1546,8 +1547,8 @@
   </sheetPr>
   <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1557,7 +1558,7 @@
     <col width="18.7109375" customWidth="1" style="15" min="3" max="3"/>
     <col width="45" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
     <col width="16.28515625" customWidth="1" style="15" min="5" max="5"/>
-    <col width="28.85546875" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
     <col width="14.5703125" customWidth="1" style="15" min="7" max="7"/>
     <col width="26.7109375" customWidth="1" style="15" min="8" max="8"/>
     <col width="33.28515625" customWidth="1" style="15" min="9" max="9"/>
@@ -1828,7 +1829,7 @@
       <c r="C2" s="31" t="n"/>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="E2" s="15" t="inlineStr">
@@ -1838,7 +1839,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="G2" s="103" t="inlineStr">
@@ -1868,7 +1869,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="M2" s="86" t="inlineStr">
@@ -1898,7 +1899,7 @@
       </c>
       <c r="R2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="S2" s="86" t="inlineStr">
@@ -1930,7 +1931,7 @@
       <c r="Y2" s="15" t="n"/>
       <c r="Z2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AA2" s="15" t="n"/>
@@ -2023,6 +2024,314 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.140625" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="43.42578125" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="33.5703125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="106" min="10" max="10"/>
+    <col width="22" bestFit="1" customWidth="1" style="106" min="11" max="11"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" style="106" min="12" max="12"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="13" max="13"/>
+    <col width="17" bestFit="1" customWidth="1" style="106" min="14" max="14"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="106" min="15" max="15"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="16" max="16"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="17" max="17"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="18" max="18"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="106" min="19" max="19"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="20" max="20"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="21" max="21"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="106" min="22" max="22"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="23" max="23"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="106" min="24" max="24"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="106" min="25" max="25"/>
+    <col width="67" bestFit="1" customWidth="1" style="106" min="26" max="26"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="87" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="87" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="90" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="90" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="87" t="inlineStr">
+        <is>
+          <t>CircleSelection_Transaction</t>
+        </is>
+      </c>
+      <c r="F1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell</t>
+        </is>
+      </c>
+      <c r="G1" s="87" t="inlineStr">
+        <is>
+          <t>LenderShare_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender</t>
+        </is>
+      </c>
+      <c r="I1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location</t>
+        </is>
+      </c>
+      <c r="J1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_LegalEntity</t>
+        </is>
+      </c>
+      <c r="K1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Location</t>
+        </is>
+      </c>
+      <c r="L1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Riskbook</t>
+        </is>
+      </c>
+      <c r="M1" s="87" t="inlineStr">
+        <is>
+          <t>Transaction_Type</t>
+        </is>
+      </c>
+      <c r="N1" s="87" t="inlineStr">
+        <is>
+          <t>AssigFeeDecision</t>
+        </is>
+      </c>
+      <c r="O1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal</t>
+        </is>
+      </c>
+      <c r="P1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee</t>
+        </is>
+      </c>
+      <c r="Q1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price</t>
+        </is>
+      </c>
+      <c r="R1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount</t>
+        </is>
+      </c>
+      <c r="S1" s="90" t="inlineStr">
+        <is>
+          <t>Expected_CloseDate</t>
+        </is>
+      </c>
+      <c r="T1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender2</t>
+        </is>
+      </c>
+      <c r="U1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location2</t>
+        </is>
+      </c>
+      <c r="V1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal2</t>
+        </is>
+      </c>
+      <c r="W1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee2</t>
+        </is>
+      </c>
+      <c r="X1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price2</t>
+        </is>
+      </c>
+      <c r="Y1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount2</t>
+        </is>
+      </c>
+      <c r="Z1" s="87" t="inlineStr">
+        <is>
+          <t>Cust_Portfolio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
+        </is>
+      </c>
+      <c r="C2" s="86" t="inlineStr">
+        <is>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>New External</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="G2" s="86" t="inlineStr">
+        <is>
+          <t>Participation</t>
+        </is>
+      </c>
+      <c r="H2" s="86" t="inlineStr">
+        <is>
+          <t>CBA OBU EXTERNAL 1513026</t>
+        </is>
+      </c>
+      <c r="I2" s="86" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="J2" s="86" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="K2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="L2" s="86" t="inlineStr">
+        <is>
+          <t>Industrials, Transport and Consumer</t>
+        </is>
+      </c>
+      <c r="M2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="N2" s="86" t="inlineStr">
+        <is>
+          <t>Split</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>30</v>
+      </c>
+      <c r="P2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>04-Nov-2020</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>EU_LENDER100</t>
+        </is>
+      </c>
+      <c r="U2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="X2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="Z2" s="111" t="inlineStr">
+        <is>
+          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="Z7" s="111" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -2510,7 +2819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2601,7 +2910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3062,7 +3371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3581,7 +3890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3860,7 +4169,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="I2" s="86" t="inlineStr">
@@ -3915,7 +4224,7 @@
       </c>
       <c r="S2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="T2" s="86" t="inlineStr">
@@ -3930,17 +4239,17 @@
       </c>
       <c r="V2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="X2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="Y2" s="86" t="inlineStr">
@@ -4036,7 +4345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4181,8 +4490,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="82"/>
-    <col width="9.140625" customWidth="1" style="68" min="83" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="87"/>
+    <col width="9.140625" customWidth="1" style="68" min="88" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -7518,17 +7827,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_06112020154352RZL</t>
+          <t>R5_11112020100838QBN</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -7648,7 +7957,7 @@
       </c>
       <c r="AE2" s="48" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AF2" s="48" t="n"/>
@@ -7757,17 +8066,17 @@
       </c>
       <c r="BJ2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BL2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BN2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BO2" s="48" t="n"/>
@@ -7803,17 +8112,17 @@
       </c>
       <c r="CJ2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CK2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CM2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CN2" s="14" t="inlineStr">
@@ -7954,7 +8263,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8226,12 +8535,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -8256,12 +8565,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -8512,7 +8821,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8660,8 +8969,8 @@
   <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8941,12 +9250,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -9027,7 +9336,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="86" t="inlineStr">
@@ -9038,12 +9347,12 @@
       <c r="X2" s="50" t="n"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AA2" s="48" t="n"/>
@@ -9076,7 +9385,7 @@
       <c r="A3" s="46" t="n"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="L3" s="46" t="n"/>
@@ -9091,7 +9400,7 @@
       <c r="A4" s="46" t="n"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="L4" s="46" t="n"/>
@@ -9243,7 +9552,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="84" t="inlineStr">

</xml_diff>

<commit_message>
GDE-8222 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="885" windowWidth="28800" windowHeight="7830" tabRatio="923" firstSheet="2" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYND02_PrimaryAllocation" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED07_UpfrontFee_Payment" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_ExternalParticipation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -298,7 +299,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -452,6 +453,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,14 +1419,14 @@
     <col width="5.85546875" bestFit="1" customWidth="1" style="88" min="1" max="1"/>
     <col width="28" bestFit="1" customWidth="1" style="88" min="2" max="2"/>
     <col width="44" bestFit="1" customWidth="1" style="88" min="3" max="3"/>
-    <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="4" max="4"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="88" min="4" max="4"/>
     <col width="21.7109375" customWidth="1" style="88" min="5" max="5"/>
     <col width="26.28515625" bestFit="1" customWidth="1" style="88" min="6" max="6"/>
     <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="7" max="7"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="88" min="8" max="8"/>
     <col width="20.5703125" customWidth="1" style="88" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="88" min="10" max="28"/>
-    <col width="8.7109375" customWidth="1" style="88" min="29" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="10" max="34"/>
+    <col width="8.7109375" customWidth="1" style="88" min="35" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -1487,12 +1489,12 @@
       </c>
       <c r="C2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -1507,7 +1509,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="88" t="inlineStr">
@@ -1521,7 +1523,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="46" t="n"/>
       <c r="B4" s="86" t="n"/>
@@ -1538,6 +1539,310 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.140625" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="43.42578125" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="33.5703125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="106" min="10" max="10"/>
+    <col width="22" bestFit="1" customWidth="1" style="106" min="11" max="11"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" style="106" min="12" max="12"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="13" max="13"/>
+    <col width="17" bestFit="1" customWidth="1" style="106" min="14" max="14"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="106" min="15" max="15"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="16" max="16"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="17" max="17"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="18" max="18"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="106" min="19" max="19"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="20" max="20"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="21" max="21"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="106" min="22" max="22"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="23" max="23"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="106" min="24" max="24"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="106" min="25" max="25"/>
+    <col width="67" bestFit="1" customWidth="1" style="106" min="26" max="26"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="87" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="87" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="90" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="90" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="87" t="inlineStr">
+        <is>
+          <t>CircleSelection_Transaction</t>
+        </is>
+      </c>
+      <c r="F1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell</t>
+        </is>
+      </c>
+      <c r="G1" s="87" t="inlineStr">
+        <is>
+          <t>LenderShare_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender</t>
+        </is>
+      </c>
+      <c r="I1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location</t>
+        </is>
+      </c>
+      <c r="J1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_LegalEntity</t>
+        </is>
+      </c>
+      <c r="K1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Location</t>
+        </is>
+      </c>
+      <c r="L1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Riskbook</t>
+        </is>
+      </c>
+      <c r="M1" s="87" t="inlineStr">
+        <is>
+          <t>Transaction_Type</t>
+        </is>
+      </c>
+      <c r="N1" s="87" t="inlineStr">
+        <is>
+          <t>AssigFeeDecision</t>
+        </is>
+      </c>
+      <c r="O1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal</t>
+        </is>
+      </c>
+      <c r="P1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee</t>
+        </is>
+      </c>
+      <c r="Q1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price</t>
+        </is>
+      </c>
+      <c r="R1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount</t>
+        </is>
+      </c>
+      <c r="S1" s="90" t="inlineStr">
+        <is>
+          <t>Expected_CloseDate</t>
+        </is>
+      </c>
+      <c r="T1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender2</t>
+        </is>
+      </c>
+      <c r="U1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location2</t>
+        </is>
+      </c>
+      <c r="V1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal2</t>
+        </is>
+      </c>
+      <c r="W1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee2</t>
+        </is>
+      </c>
+      <c r="X1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price2</t>
+        </is>
+      </c>
+      <c r="Y1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount2</t>
+        </is>
+      </c>
+      <c r="Z1" s="87" t="inlineStr">
+        <is>
+          <t>Cust_Portfolio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
+        </is>
+      </c>
+      <c r="C2" s="86" t="inlineStr">
+        <is>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>New External</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="G2" s="86" t="inlineStr">
+        <is>
+          <t>Participation</t>
+        </is>
+      </c>
+      <c r="H2" s="86" t="inlineStr">
+        <is>
+          <t>CBA OBU EXTERNAL 1513026</t>
+        </is>
+      </c>
+      <c r="I2" s="86" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="J2" s="86" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="K2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="L2" s="86" t="inlineStr">
+        <is>
+          <t>Industrials, Transport and Consumer</t>
+        </is>
+      </c>
+      <c r="M2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="N2" s="86" t="inlineStr">
+        <is>
+          <t>Split</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>30</v>
+      </c>
+      <c r="P2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>04-Nov-2020</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>EU_LENDER100</t>
+        </is>
+      </c>
+      <c r="U2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="X2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="Z2" s="111" t="inlineStr">
+        <is>
+          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="Z7" s="111" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor theme="9" tint="0.3999755851924192"/>
@@ -1557,13 +1862,13 @@
     <col width="18.7109375" customWidth="1" style="15" min="3" max="3"/>
     <col width="45" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
     <col width="16.28515625" customWidth="1" style="15" min="5" max="5"/>
-    <col width="28.85546875" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
     <col width="14.5703125" customWidth="1" style="15" min="7" max="7"/>
     <col width="26.7109375" customWidth="1" style="15" min="8" max="8"/>
     <col width="33.28515625" customWidth="1" style="15" min="9" max="9"/>
     <col width="21.7109375" customWidth="1" style="15" min="10" max="10"/>
     <col width="17.42578125" customWidth="1" style="15" min="11" max="11"/>
-    <col width="21.140625" customWidth="1" style="15" min="12" max="12"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="15" min="12" max="12"/>
     <col width="10.42578125" customWidth="1" style="15" min="13" max="13"/>
     <col width="18.5703125" customWidth="1" style="15" min="14" max="14"/>
     <col width="14.140625" customWidth="1" style="15" min="15" max="15"/>
@@ -1828,7 +2133,7 @@
       <c r="C2" s="31" t="n"/>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="E2" s="15" t="inlineStr">
@@ -1838,7 +2143,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="G2" s="103" t="inlineStr">
@@ -1846,12 +2151,12 @@
           <t>3</t>
         </is>
       </c>
-      <c r="H2" s="86" t="inlineStr">
-        <is>
-          <t>20,000,000.00</t>
-        </is>
-      </c>
-      <c r="I2" s="86" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>100,000,000.00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
@@ -1868,12 +2173,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="M2" s="86" t="inlineStr">
         <is>
-          <t>60000581</t>
+          <t>60000790</t>
         </is>
       </c>
       <c r="N2" s="15" t="inlineStr">
@@ -1888,7 +2193,7 @@
       </c>
       <c r="P2" s="103" t="inlineStr">
         <is>
-          <t>20000000.00</t>
+          <t>60000000.00</t>
         </is>
       </c>
       <c r="Q2" s="15" t="inlineStr">
@@ -1898,7 +2203,7 @@
       </c>
       <c r="R2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="S2" s="86" t="inlineStr">
@@ -1930,7 +2235,7 @@
       <c r="Y2" s="15" t="n"/>
       <c r="Z2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AA2" s="15" t="n"/>
@@ -1956,7 +2261,7 @@
       <c r="AN2" s="32" t="n"/>
       <c r="AO2" s="86" t="inlineStr">
         <is>
-          <t>CG852/Hold for Investment - Europe/NR_PRF</t>
+          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
         </is>
       </c>
       <c r="AQ2" s="86" t="inlineStr">
@@ -2020,7 +2325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2510,7 +2815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2601,7 +2906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3062,7 +3367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3402,7 +3707,7 @@
       </c>
       <c r="K2" s="86" t="inlineStr">
         <is>
-          <t>08-Sep-2020</t>
+          <t>04-Dec-2020</t>
         </is>
       </c>
       <c r="L2" s="15" t="inlineStr">
@@ -3571,6 +3876,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="N4" s="44" t="n"/>
     </row>
@@ -3581,7 +3887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3860,7 +4166,7 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="I2" s="86" t="inlineStr">
@@ -3915,7 +4221,7 @@
       </c>
       <c r="S2" s="86" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="T2" s="86" t="inlineStr">
@@ -3930,17 +4236,17 @@
       </c>
       <c r="V2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="X2" s="86" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="Y2" s="86" t="inlineStr">
@@ -4036,7 +4342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4181,8 +4487,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="82"/>
-    <col width="9.140625" customWidth="1" style="68" min="83" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="88"/>
+    <col width="9.140625" customWidth="1" style="68" min="89" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -7518,17 +7824,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_06112020154352RZL</t>
+          <t>R5_11112020100838QBN</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -7648,7 +7954,7 @@
       </c>
       <c r="AE2" s="48" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AF2" s="48" t="n"/>
@@ -7757,17 +8063,17 @@
       </c>
       <c r="BJ2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BL2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BN2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="BO2" s="48" t="n"/>
@@ -7803,17 +8109,17 @@
       </c>
       <c r="CJ2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CK2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CM2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="CN2" s="14" t="inlineStr">
@@ -7954,7 +8260,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8226,12 +8532,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
@@ -8256,12 +8562,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -8512,7 +8818,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="D2" s="22" t="inlineStr">
@@ -8660,8 +8966,8 @@
   <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8941,12 +9247,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="86" t="inlineStr">
         <is>
-          <t>R5_BYBK_100M_06112020160123XRR</t>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
         </is>
       </c>
       <c r="E2" s="86" t="inlineStr">
@@ -9027,7 +9333,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="W2" s="86" t="inlineStr">
@@ -9038,12 +9344,12 @@
       <c r="X2" s="50" t="n"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>03-Nov-2020</t>
+          <t>04-Nov-2020</t>
         </is>
       </c>
       <c r="AA2" s="48" t="n"/>
@@ -9076,7 +9382,7 @@
       <c r="A3" s="46" t="n"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="L3" s="46" t="n"/>
@@ -9091,7 +9397,7 @@
       <c r="A4" s="46" t="n"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="L4" s="46" t="n"/>
@@ -9243,7 +9549,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PRTCPTION_BYBCK100M_06112020154348IMA</t>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
         </is>
       </c>
       <c r="D2" s="84" t="inlineStr">

</xml_diff>

<commit_message>
GDE-8223 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="11" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="5" activeTab="12" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_ExternalParticipation" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO05_ExtParticipationBuyBack" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1425,8 +1426,8 @@
     <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="7" max="7"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="88" min="8" max="8"/>
     <col width="20.5703125" customWidth="1" style="88" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="88" min="10" max="34"/>
-    <col width="8.7109375" customWidth="1" style="88" min="35" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="10" max="38"/>
+    <col width="8.7109375" customWidth="1" style="88" min="39" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -1547,8 +1548,8 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1851,8 +1852,8 @@
   </sheetPr>
   <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2328,6 +2329,349 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AC7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.140625" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="43.42578125" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="33.5703125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="106" min="10" max="10"/>
+    <col width="22" bestFit="1" customWidth="1" style="106" min="11" max="11"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" style="106" min="12" max="12"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="13" max="13"/>
+    <col width="17" bestFit="1" customWidth="1" style="106" min="14" max="14"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="106" min="15" max="15"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="16" max="16"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="17" max="17"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="18" max="18"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="106" min="19" max="19"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="20" max="20"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="21" max="21"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="106" min="22" max="22"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="23" max="23"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="106" min="24" max="24"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="106" min="25" max="25"/>
+    <col width="67" bestFit="1" customWidth="1" style="106" min="26" max="26"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="106" min="27" max="27"/>
+    <col width="20" bestFit="1" customWidth="1" style="106" min="28" max="28"/>
+    <col width="40.7109375" bestFit="1" customWidth="1" style="106" min="29" max="29"/>
+    <col width="9.140625" customWidth="1" style="106" min="30" max="31"/>
+    <col width="9.140625" customWidth="1" style="106" min="32" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="87" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="87" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="90" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="90" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="87" t="inlineStr">
+        <is>
+          <t>CircleSelection_Transaction</t>
+        </is>
+      </c>
+      <c r="F1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell</t>
+        </is>
+      </c>
+      <c r="G1" s="87" t="inlineStr">
+        <is>
+          <t>LenderShare_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Lender</t>
+        </is>
+      </c>
+      <c r="I1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Location</t>
+        </is>
+      </c>
+      <c r="J1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender</t>
+        </is>
+      </c>
+      <c r="K1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location</t>
+        </is>
+      </c>
+      <c r="L1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Riskbook</t>
+        </is>
+      </c>
+      <c r="M1" s="87" t="inlineStr">
+        <is>
+          <t>Transaction_Type</t>
+        </is>
+      </c>
+      <c r="N1" s="87" t="inlineStr">
+        <is>
+          <t>AssigFeeDecision</t>
+        </is>
+      </c>
+      <c r="O1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal</t>
+        </is>
+      </c>
+      <c r="P1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee</t>
+        </is>
+      </c>
+      <c r="Q1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price</t>
+        </is>
+      </c>
+      <c r="R1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount</t>
+        </is>
+      </c>
+      <c r="S1" s="90" t="inlineStr">
+        <is>
+          <t>Expected_CloseDate</t>
+        </is>
+      </c>
+      <c r="T1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender2</t>
+        </is>
+      </c>
+      <c r="U1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location2</t>
+        </is>
+      </c>
+      <c r="V1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal2</t>
+        </is>
+      </c>
+      <c r="W1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee2</t>
+        </is>
+      </c>
+      <c r="X1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price2</t>
+        </is>
+      </c>
+      <c r="Y1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount2</t>
+        </is>
+      </c>
+      <c r="Z1" s="87" t="inlineStr">
+        <is>
+          <t>Cust_Portfolio</t>
+        </is>
+      </c>
+      <c r="AA1" s="89" t="inlineStr">
+        <is>
+          <t>Buyer_Portfolio</t>
+        </is>
+      </c>
+      <c r="AB1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_ExpenseCode</t>
+        </is>
+      </c>
+      <c r="AC1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Branch</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
+        </is>
+      </c>
+      <c r="C2" s="86" t="inlineStr">
+        <is>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>New External</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="G2" s="86" t="inlineStr">
+        <is>
+          <t>Participation</t>
+        </is>
+      </c>
+      <c r="H2" s="86" t="inlineStr">
+        <is>
+          <t>CBA OBU EXTERNAL 1513026</t>
+        </is>
+      </c>
+      <c r="I2" s="86" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="J2" s="86" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="K2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="L2" s="86" t="inlineStr">
+        <is>
+          <t>Industrials, Transport and Consumer</t>
+        </is>
+      </c>
+      <c r="M2" s="86" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="N2" s="86" t="inlineStr">
+        <is>
+          <t>Split</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>30</v>
+      </c>
+      <c r="P2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>100</v>
+      </c>
+      <c r="R2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>04-Nov-2020</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>EU_LENDER100</t>
+        </is>
+      </c>
+      <c r="U2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="X2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="Z2" s="111" t="inlineStr">
+        <is>
+          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+        </is>
+      </c>
+      <c r="AA2" s="88" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Europe</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>IT_SAF</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - Amsterdam</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="Z7" s="111" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -2815,7 +3159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2906,7 +3250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3367,7 +3711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3876,7 +4220,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="N4" s="44" t="n"/>
     </row>
@@ -3887,7 +4230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4342,7 +4685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4487,8 +4830,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="88"/>
-    <col width="9.140625" customWidth="1" style="68" min="89" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="92"/>
+    <col width="9.140625" customWidth="1" style="68" min="93" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">

</xml_diff>

<commit_message>
GDE-8224 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S5_EU_S5_RPA_Buyback.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="5" activeTab="12" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="8" activeTab="13" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_ExternalParticipation" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO05_ExtParticipationBuyBack" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO06_InternalParticipation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -300,7 +301,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -455,6 +456,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1426,8 +1429,8 @@
     <col width="32.28515625" bestFit="1" customWidth="1" style="88" min="7" max="7"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="88" min="8" max="8"/>
     <col width="20.5703125" customWidth="1" style="88" min="9" max="9"/>
-    <col width="8.7109375" customWidth="1" style="88" min="10" max="38"/>
-    <col width="8.7109375" customWidth="1" style="88" min="39" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="10" max="39"/>
+    <col width="8.7109375" customWidth="1" style="88" min="40" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -2335,8 +2338,8 @@
   </sheetPr>
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2370,8 +2373,8 @@
     <col width="26.28515625" bestFit="1" customWidth="1" style="106" min="27" max="27"/>
     <col width="20" bestFit="1" customWidth="1" style="106" min="28" max="28"/>
     <col width="40.7109375" bestFit="1" customWidth="1" style="106" min="29" max="29"/>
-    <col width="9.140625" customWidth="1" style="106" min="30" max="31"/>
-    <col width="9.140625" customWidth="1" style="106" min="32" max="16384"/>
+    <col width="9.140625" customWidth="1" style="106" min="30" max="32"/>
+    <col width="9.140625" customWidth="1" style="106" min="33" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2656,10 +2659,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
     <row r="7">
       <c r="Z7" s="111" t="n"/>
     </row>
@@ -2670,6 +2669,359 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.140625" bestFit="1" customWidth="1" style="106" min="1" max="1"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="106" min="2" max="2"/>
+    <col width="43.85546875" bestFit="1" customWidth="1" style="106" min="3" max="3"/>
+    <col width="34.42578125" bestFit="1" customWidth="1" style="106" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" style="106" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" style="106" min="6" max="6"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="106" min="7" max="7"/>
+    <col width="31.42578125" bestFit="1" customWidth="1" style="106" min="8" max="8"/>
+    <col width="21" bestFit="1" customWidth="1" style="106" min="9" max="9"/>
+    <col width="21" customWidth="1" style="106" min="10" max="10"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="106" min="11" max="11"/>
+    <col width="22" bestFit="1" customWidth="1" style="106" min="12" max="12"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" style="106" min="13" max="13"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="14" max="14"/>
+    <col width="17" bestFit="1" customWidth="1" style="106" min="15" max="15"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="106" min="16" max="16"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="17" max="17"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="106" min="18" max="18"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="106" min="19" max="19"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="106" min="20" max="20"/>
+    <col width="15.140625" bestFit="1" customWidth="1" style="106" min="21" max="21"/>
+    <col width="22" bestFit="1" customWidth="1" style="106" min="22" max="22"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="106" min="23" max="23"/>
+    <col width="20.5703125" bestFit="1" customWidth="1" style="106" min="24" max="24"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="106" min="25" max="25"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="106" min="26" max="26"/>
+    <col width="38.28515625" bestFit="1" customWidth="1" style="106" min="27" max="27"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="106" min="28" max="28"/>
+    <col width="20" bestFit="1" customWidth="1" style="106" min="29" max="29"/>
+    <col width="35" bestFit="1" customWidth="1" style="106" min="30" max="30"/>
+    <col width="9.140625" customWidth="1" style="106" min="31" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="87" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="87" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="90" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="90" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="87" t="inlineStr">
+        <is>
+          <t>CircleSelection_Transaction</t>
+        </is>
+      </c>
+      <c r="F1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell</t>
+        </is>
+      </c>
+      <c r="G1" s="87" t="inlineStr">
+        <is>
+          <t>LenderShare_Type</t>
+        </is>
+      </c>
+      <c r="H1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Lender</t>
+        </is>
+      </c>
+      <c r="I1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Location</t>
+        </is>
+      </c>
+      <c r="J1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_RiskBook</t>
+        </is>
+      </c>
+      <c r="K1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_LegalEntity</t>
+        </is>
+      </c>
+      <c r="L1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_Location</t>
+        </is>
+      </c>
+      <c r="M1" s="87" t="inlineStr">
+        <is>
+          <t>Seller_RiskBook</t>
+        </is>
+      </c>
+      <c r="N1" s="87" t="inlineStr">
+        <is>
+          <t>Transaction_Type</t>
+        </is>
+      </c>
+      <c r="O1" s="87" t="inlineStr">
+        <is>
+          <t>AssigFeeDecision</t>
+        </is>
+      </c>
+      <c r="P1" s="87" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal</t>
+        </is>
+      </c>
+      <c r="Q1" s="87" t="inlineStr">
+        <is>
+          <t>Int_Fee</t>
+        </is>
+      </c>
+      <c r="R1" s="87" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price</t>
+        </is>
+      </c>
+      <c r="S1" s="90" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount</t>
+        </is>
+      </c>
+      <c r="T1" s="112" t="inlineStr">
+        <is>
+          <t>Expected_CloseDate</t>
+        </is>
+      </c>
+      <c r="U1" s="112" t="inlineStr">
+        <is>
+          <t>Buyer_Lender2</t>
+        </is>
+      </c>
+      <c r="V1" s="112" t="inlineStr">
+        <is>
+          <t>Buyer_Location2</t>
+        </is>
+      </c>
+      <c r="W1" s="112" t="inlineStr">
+        <is>
+          <t>Pct_of_Deal2</t>
+        </is>
+      </c>
+      <c r="X1" s="112" t="inlineStr">
+        <is>
+          <t>Int_Fee2</t>
+        </is>
+      </c>
+      <c r="Y1" s="112" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Price2</t>
+        </is>
+      </c>
+      <c r="Z1" s="112" t="inlineStr">
+        <is>
+          <t>Buy_Sell_Amount2</t>
+        </is>
+      </c>
+      <c r="AA1" s="87" t="inlineStr">
+        <is>
+          <t>Cust_Portfolio</t>
+        </is>
+      </c>
+      <c r="AB1" s="89" t="inlineStr">
+        <is>
+          <t>Buyer_Portfolio</t>
+        </is>
+      </c>
+      <c r="AC1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_ExpenseCode</t>
+        </is>
+      </c>
+      <c r="AD1" s="87" t="inlineStr">
+        <is>
+          <t>Buyer_Branch</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_S5_EU_S5_RPA_Buyback</t>
+        </is>
+      </c>
+      <c r="C2" s="86" t="inlineStr">
+        <is>
+          <t>PRTCPTION_BYBCK100M_11112020100835MQG</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R5_BYBK_100M_11112020102708NXK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>New Internal</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="G2" s="86" t="inlineStr">
+        <is>
+          <t>Participation</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AU-OBU</t>
+        </is>
+      </c>
+      <c r="I2" s="86" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="J2" s="86" t="inlineStr">
+        <is>
+          <t>Debt Markets</t>
+        </is>
+      </c>
+      <c r="K2" s="86" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="L2" s="86" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="M2" s="86" t="inlineStr">
+        <is>
+          <t>Industrials, Transport and Consumer</t>
+        </is>
+      </c>
+      <c r="N2" s="86" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="O2" s="86" t="inlineStr">
+        <is>
+          <t>Split</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="86" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>100</v>
+      </c>
+      <c r="S2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="T2" s="113" t="inlineStr">
+        <is>
+          <t>04-Nov-2020</t>
+        </is>
+      </c>
+      <c r="U2" s="113" t="inlineStr">
+        <is>
+          <t>EU_LENDER100</t>
+        </is>
+      </c>
+      <c r="V2" s="48" t="inlineStr">
+        <is>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="W2" s="113" t="n">
+        <v>20</v>
+      </c>
+      <c r="X2" s="48" t="inlineStr">
+        <is>
+          <t>Actual\Settlement Date</t>
+        </is>
+      </c>
+      <c r="Y2" s="113" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z2" s="113" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="AA2" s="111" t="inlineStr">
+        <is>
+          <t>CG852/Hold for Investment - Europe/IT_SAF</t>
+        </is>
+      </c>
+      <c r="AB2" s="88" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>DM_CFS</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - OBU</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="AA7" s="111" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3159,7 +3511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3250,7 +3602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3711,7 +4063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4230,7 +4582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4677,97 +5029,6 @@
       <c r="AA5" s="11" t="n"/>
       <c r="AB5" s="11" t="n"/>
       <c r="AC5" s="11" t="n"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
-  <cols>
-    <col width="6.140625" customWidth="1" style="86" min="1" max="1"/>
-    <col width="43.28515625" customWidth="1" style="86" min="2" max="2"/>
-    <col width="24.28515625" customWidth="1" style="86" min="3" max="3"/>
-    <col width="11.42578125" customWidth="1" style="3" min="4" max="4"/>
-    <col width="20.85546875" customWidth="1" style="86" min="5" max="5"/>
-    <col width="15.28515625" customWidth="1" style="86" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="12" t="inlineStr">
-        <is>
-          <t>rowid</t>
-        </is>
-      </c>
-      <c r="B1" s="12" t="inlineStr">
-        <is>
-          <t>Test_Case</t>
-        </is>
-      </c>
-      <c r="C1" s="13" t="inlineStr">
-        <is>
-          <t>Deal_Name</t>
-        </is>
-      </c>
-      <c r="D1" s="28" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Financial_Ratio_Type</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Financial_Ratio</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" customFormat="1" s="86">
-      <c r="A2" s="86" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" s="86" t="inlineStr">
-        <is>
-          <t>EVGLIQ_AMD_DLCH01 Deal Change Transaction</t>
-        </is>
-      </c>
-      <c r="C2" s="86" t="inlineStr">
-        <is>
-          <t>CBAEU_10062020125653TLE</t>
-        </is>
-      </c>
-      <c r="D2" s="86" t="inlineStr">
-        <is>
-          <t>22-May-2020</t>
-        </is>
-      </c>
-      <c r="E2" s="86" t="inlineStr">
-        <is>
-          <t>ICR</t>
-        </is>
-      </c>
-      <c r="F2" s="86" t="n">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4830,8 +5091,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="92"/>
-    <col width="9.140625" customWidth="1" style="68" min="93" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="93"/>
+    <col width="9.140625" customWidth="1" style="68" min="94" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -5295,6 +5556,97 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup orientation="portrait" paperSize="9" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="6.140625" customWidth="1" style="86" min="1" max="1"/>
+    <col width="43.28515625" customWidth="1" style="86" min="2" max="2"/>
+    <col width="24.28515625" customWidth="1" style="86" min="3" max="3"/>
+    <col width="11.42578125" customWidth="1" style="3" min="4" max="4"/>
+    <col width="20.85546875" customWidth="1" style="86" min="5" max="5"/>
+    <col width="15.28515625" customWidth="1" style="86" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="12" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="12" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="13" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="28" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Financial_Ratio_Type</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Financial_Ratio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="86">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVGLIQ_AMD_DLCH01 Deal Change Transaction</t>
+        </is>
+      </c>
+      <c r="C2" s="86" t="inlineStr">
+        <is>
+          <t>CBAEU_10062020125653TLE</t>
+        </is>
+      </c>
+      <c r="D2" s="86" t="inlineStr">
+        <is>
+          <t>22-May-2020</t>
+        </is>
+      </c>
+      <c r="E2" s="86" t="inlineStr">
+        <is>
+          <t>ICR</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 

</xml_diff>